<commit_message>
Gannt Prevetivo e Consuntivo 22.12.2017
</commit_message>
<xml_diff>
--- a/Analisi e Gannt.xlsx
+++ b/Analisi e Gannt.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\scuola\terzo_anno\Primo semestre\Mod. 306\Progetto 2 - locale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scuola\TerzoAnno\Progetto\Progetto2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -279,7 +279,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1043,7 +1043,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1223,6 +1223,67 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1235,65 +1296,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1301,6 +1314,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1334,64 +1392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1705,71 +1706,71 @@
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="146"/>
-      <c r="C2" s="147"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="130"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="148"/>
-      <c r="B3" s="149"/>
-      <c r="C3" s="150"/>
+      <c r="A3" s="131"/>
+      <c r="B3" s="132"/>
+      <c r="C3" s="133"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="137" t="s">
+      <c r="B5" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="138"/>
+      <c r="C5" s="135"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="131" t="s">
+      <c r="B6" s="138" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="132"/>
+      <c r="C6" s="139"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="131">
+      <c r="B7" s="138">
         <v>1</v>
       </c>
-      <c r="C7" s="132"/>
+      <c r="C7" s="139"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="132"/>
+      <c r="C8" s="139"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="131" t="s">
+      <c r="B9" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="132"/>
+      <c r="C9" s="139"/>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="133" t="s">
+      <c r="B10" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="134"/>
+      <c r="C10" s="137"/>
     </row>
     <row r="11" spans="1:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
@@ -1781,30 +1782,30 @@
       <c r="A12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="143" t="s">
+      <c r="B12" s="144" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="144"/>
+      <c r="C12" s="145"/>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="141" t="s">
+      <c r="B13" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="142"/>
+      <c r="C13" s="143"/>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="139" t="s">
+      <c r="B14" s="140" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="140"/>
+      <c r="C14" s="141"/>
       <c r="D14"/>
     </row>
     <row r="15" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1816,60 +1817,60 @@
       <c r="A16" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="137" t="s">
+      <c r="B16" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="138"/>
+      <c r="C16" s="135"/>
       <c r="D16"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="131" t="s">
+      <c r="B17" s="138" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="132"/>
+      <c r="C17" s="139"/>
       <c r="D17"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="131">
+      <c r="B18" s="138">
         <v>1</v>
       </c>
-      <c r="C18" s="132"/>
+      <c r="C18" s="139"/>
       <c r="D18"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="132"/>
+      <c r="C19" s="139"/>
       <c r="D19"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="131" t="s">
+      <c r="B20" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="132"/>
+      <c r="C20" s="139"/>
       <c r="D20"/>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="133" t="s">
+      <c r="B21" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="134"/>
+      <c r="C21" s="137"/>
       <c r="D21"/>
     </row>
     <row r="22" spans="1:5" ht="3.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1882,40 +1883,40 @@
       <c r="A23" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="135" t="s">
+      <c r="B23" s="146" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="136"/>
+      <c r="C23" s="147"/>
       <c r="D23"/>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="127" t="s">
+      <c r="B24" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="128"/>
+      <c r="C24" s="149"/>
       <c r="D24"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="127" t="s">
+      <c r="B25" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="128"/>
+      <c r="C25" s="149"/>
       <c r="D25"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="129" t="s">
+      <c r="B26" s="150" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="130"/>
+      <c r="C26" s="151"/>
       <c r="D26"/>
     </row>
     <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1925,20 +1926,20 @@
       <c r="A28" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="137" t="s">
+      <c r="B28" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="138"/>
+      <c r="C28" s="135"/>
       <c r="D28"/>
     </row>
     <row r="29" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="131" t="s">
+      <c r="B29" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="132"/>
+      <c r="C29" s="139"/>
       <c r="D29"/>
       <c r="E29"/>
     </row>
@@ -1946,10 +1947,10 @@
       <c r="A30" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="131">
+      <c r="B30" s="138">
         <v>1</v>
       </c>
-      <c r="C30" s="132"/>
+      <c r="C30" s="139"/>
       <c r="D30"/>
       <c r="E30"/>
     </row>
@@ -1957,10 +1958,10 @@
       <c r="A31" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="131" t="s">
+      <c r="B31" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="132"/>
+      <c r="C31" s="139"/>
       <c r="D31"/>
       <c r="E31"/>
     </row>
@@ -1968,20 +1969,20 @@
       <c r="A32" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="131" t="s">
+      <c r="B32" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="132"/>
+      <c r="C32" s="139"/>
       <c r="D32"/>
     </row>
     <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="133" t="s">
+      <c r="B33" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="134"/>
+      <c r="C33" s="137"/>
       <c r="D33"/>
     </row>
     <row r="34" spans="1:5" ht="2.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1994,37 +1995,37 @@
       <c r="A35" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="135" t="s">
+      <c r="B35" s="146" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="136"/>
+      <c r="C35" s="147"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="127" t="s">
+      <c r="B36" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="128"/>
+      <c r="C36" s="149"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="127" t="s">
+      <c r="B37" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="128"/>
+      <c r="C37" s="149"/>
     </row>
     <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="129" t="s">
+      <c r="B38" s="150" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="130"/>
+      <c r="C38" s="151"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39"/>
@@ -2144,18 +2145,14 @@
     <row r="68" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
@@ -2166,14 +2163,18 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2187,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AJ78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W59" sqref="W59"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V50" sqref="V50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2278,7 +2279,7 @@
       <c r="AF2" s="79">
         <v>3</v>
       </c>
-      <c r="AG2" s="181"/>
+      <c r="AG2" s="155"/>
       <c r="AH2" s="69" t="s">
         <v>73</v>
       </c>
@@ -2308,47 +2309,47 @@
       <c r="H3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="177">
+      <c r="I3" s="162">
         <v>43049</v>
       </c>
-      <c r="J3" s="175"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="174">
+      <c r="J3" s="159"/>
+      <c r="K3" s="160"/>
+      <c r="L3" s="158">
         <v>43056</v>
       </c>
-      <c r="M3" s="175"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="174">
+      <c r="M3" s="159"/>
+      <c r="N3" s="160"/>
+      <c r="O3" s="158">
         <v>43063</v>
       </c>
-      <c r="P3" s="175"/>
-      <c r="Q3" s="176"/>
-      <c r="R3" s="174">
+      <c r="P3" s="159"/>
+      <c r="Q3" s="160"/>
+      <c r="R3" s="158">
         <v>43070</v>
       </c>
-      <c r="S3" s="175"/>
-      <c r="T3" s="176"/>
-      <c r="U3" s="174">
+      <c r="S3" s="159"/>
+      <c r="T3" s="160"/>
+      <c r="U3" s="158">
         <v>43084</v>
       </c>
-      <c r="V3" s="175"/>
-      <c r="W3" s="176"/>
-      <c r="X3" s="174">
+      <c r="V3" s="159"/>
+      <c r="W3" s="160"/>
+      <c r="X3" s="158">
         <v>43091</v>
       </c>
-      <c r="Y3" s="175"/>
-      <c r="Z3" s="176"/>
-      <c r="AA3" s="174">
+      <c r="Y3" s="159"/>
+      <c r="Z3" s="160"/>
+      <c r="AA3" s="158">
         <v>43112</v>
       </c>
-      <c r="AB3" s="175"/>
-      <c r="AC3" s="176"/>
-      <c r="AD3" s="175">
+      <c r="AB3" s="159"/>
+      <c r="AC3" s="160"/>
+      <c r="AD3" s="159">
         <v>43119</v>
       </c>
-      <c r="AE3" s="175"/>
-      <c r="AF3" s="182"/>
-      <c r="AG3" s="181"/>
+      <c r="AE3" s="159"/>
+      <c r="AF3" s="161"/>
+      <c r="AG3" s="155"/>
       <c r="AH3" s="70" t="s">
         <v>74</v>
       </c>
@@ -2360,41 +2361,41 @@
       </c>
     </row>
     <row r="4" spans="2:36" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="158" t="s">
+      <c r="B4" s="178" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="159"/>
-      <c r="D4" s="159"/>
-      <c r="E4" s="159"/>
-      <c r="F4" s="160"/>
+      <c r="C4" s="179"/>
+      <c r="D4" s="179"/>
+      <c r="E4" s="179"/>
+      <c r="F4" s="180"/>
       <c r="H4" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="151"/>
-      <c r="J4" s="151"/>
-      <c r="K4" s="151"/>
-      <c r="L4" s="151"/>
-      <c r="M4" s="151"/>
-      <c r="N4" s="151"/>
-      <c r="O4" s="151"/>
-      <c r="P4" s="151"/>
-      <c r="Q4" s="151"/>
-      <c r="R4" s="151"/>
-      <c r="S4" s="151"/>
-      <c r="T4" s="151"/>
-      <c r="U4" s="151"/>
-      <c r="V4" s="151"/>
-      <c r="W4" s="151"/>
-      <c r="X4" s="151"/>
-      <c r="Y4" s="151"/>
-      <c r="Z4" s="151"/>
-      <c r="AA4" s="151"/>
-      <c r="AB4" s="151"/>
-      <c r="AC4" s="151"/>
-      <c r="AD4" s="151"/>
-      <c r="AE4" s="151"/>
-      <c r="AF4" s="152"/>
-      <c r="AG4" s="181"/>
+      <c r="I4" s="156"/>
+      <c r="J4" s="156"/>
+      <c r="K4" s="156"/>
+      <c r="L4" s="156"/>
+      <c r="M4" s="156"/>
+      <c r="N4" s="156"/>
+      <c r="O4" s="156"/>
+      <c r="P4" s="156"/>
+      <c r="Q4" s="156"/>
+      <c r="R4" s="156"/>
+      <c r="S4" s="156"/>
+      <c r="T4" s="156"/>
+      <c r="U4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="156"/>
+      <c r="Z4" s="156"/>
+      <c r="AA4" s="156"/>
+      <c r="AB4" s="156"/>
+      <c r="AC4" s="156"/>
+      <c r="AD4" s="156"/>
+      <c r="AE4" s="156"/>
+      <c r="AF4" s="157"/>
+      <c r="AG4" s="155"/>
       <c r="AH4" s="71" t="s">
         <v>75</v>
       </c>
@@ -2440,7 +2441,7 @@
       <c r="AD5" s="43"/>
       <c r="AE5" s="43"/>
       <c r="AF5" s="44"/>
-      <c r="AG5" s="181"/>
+      <c r="AG5" s="155"/>
     </row>
     <row r="6" spans="2:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="16" t="s">
@@ -2477,11 +2478,11 @@
       <c r="AD6" s="30"/>
       <c r="AE6" s="30"/>
       <c r="AF6" s="31"/>
-      <c r="AG6" s="181"/>
-      <c r="AI6" s="153" t="s">
+      <c r="AG6" s="155"/>
+      <c r="AI6" s="173" t="s">
         <v>39</v>
       </c>
-      <c r="AJ6" s="154"/>
+      <c r="AJ6" s="174"/>
     </row>
     <row r="7" spans="2:36" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="26" t="s">
@@ -2518,7 +2519,7 @@
       <c r="AD7" s="40"/>
       <c r="AE7" s="40"/>
       <c r="AF7" s="41"/>
-      <c r="AG7" s="181"/>
+      <c r="AG7" s="155"/>
       <c r="AI7" s="20" t="s">
         <v>40</v>
       </c>
@@ -2527,41 +2528,41 @@
       </c>
     </row>
     <row r="8" spans="2:36" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="161" t="s">
+      <c r="B8" s="181" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="162"/>
-      <c r="D8" s="162"/>
-      <c r="E8" s="162"/>
-      <c r="F8" s="163"/>
+      <c r="C8" s="182"/>
+      <c r="D8" s="182"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="183"/>
       <c r="H8" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="151"/>
-      <c r="J8" s="151"/>
-      <c r="K8" s="151"/>
-      <c r="L8" s="151"/>
-      <c r="M8" s="151"/>
-      <c r="N8" s="151"/>
-      <c r="O8" s="151"/>
-      <c r="P8" s="151"/>
-      <c r="Q8" s="151"/>
-      <c r="R8" s="151"/>
-      <c r="S8" s="151"/>
-      <c r="T8" s="151"/>
-      <c r="U8" s="151"/>
-      <c r="V8" s="151"/>
-      <c r="W8" s="151"/>
-      <c r="X8" s="151"/>
-      <c r="Y8" s="151"/>
-      <c r="Z8" s="151"/>
-      <c r="AA8" s="151"/>
-      <c r="AB8" s="151"/>
-      <c r="AC8" s="151"/>
-      <c r="AD8" s="151"/>
-      <c r="AE8" s="151"/>
-      <c r="AF8" s="152"/>
-      <c r="AG8" s="181"/>
+      <c r="I8" s="156"/>
+      <c r="J8" s="156"/>
+      <c r="K8" s="156"/>
+      <c r="L8" s="156"/>
+      <c r="M8" s="156"/>
+      <c r="N8" s="156"/>
+      <c r="O8" s="156"/>
+      <c r="P8" s="156"/>
+      <c r="Q8" s="156"/>
+      <c r="R8" s="156"/>
+      <c r="S8" s="156"/>
+      <c r="T8" s="156"/>
+      <c r="U8" s="156"/>
+      <c r="V8" s="156"/>
+      <c r="W8" s="156"/>
+      <c r="X8" s="156"/>
+      <c r="Y8" s="156"/>
+      <c r="Z8" s="156"/>
+      <c r="AA8" s="156"/>
+      <c r="AB8" s="156"/>
+      <c r="AC8" s="156"/>
+      <c r="AD8" s="156"/>
+      <c r="AE8" s="156"/>
+      <c r="AF8" s="157"/>
+      <c r="AG8" s="155"/>
       <c r="AI8" s="17" t="s">
         <v>42</v>
       </c>
@@ -2604,7 +2605,7 @@
       <c r="AD9" s="40"/>
       <c r="AE9" s="40"/>
       <c r="AF9" s="41"/>
-      <c r="AG9" s="181"/>
+      <c r="AG9" s="155"/>
       <c r="AI9" s="18" t="s">
         <v>44</v>
       </c>
@@ -2613,41 +2614,41 @@
       </c>
     </row>
     <row r="10" spans="2:36" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="155" t="s">
+      <c r="B10" s="175" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="156"/>
-      <c r="D10" s="156"/>
-      <c r="E10" s="156"/>
-      <c r="F10" s="157"/>
+      <c r="C10" s="176"/>
+      <c r="D10" s="176"/>
+      <c r="E10" s="176"/>
+      <c r="F10" s="177"/>
       <c r="H10" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="151"/>
-      <c r="J10" s="151"/>
-      <c r="K10" s="151"/>
-      <c r="L10" s="151"/>
-      <c r="M10" s="151"/>
-      <c r="N10" s="151"/>
-      <c r="O10" s="151"/>
-      <c r="P10" s="151"/>
-      <c r="Q10" s="151"/>
-      <c r="R10" s="151"/>
-      <c r="S10" s="151"/>
-      <c r="T10" s="151"/>
-      <c r="U10" s="151"/>
-      <c r="V10" s="151"/>
-      <c r="W10" s="151"/>
-      <c r="X10" s="151"/>
-      <c r="Y10" s="151"/>
-      <c r="Z10" s="151"/>
-      <c r="AA10" s="151"/>
-      <c r="AB10" s="151"/>
-      <c r="AC10" s="151"/>
-      <c r="AD10" s="151"/>
-      <c r="AE10" s="151"/>
-      <c r="AF10" s="152"/>
-      <c r="AG10" s="181"/>
+      <c r="I10" s="156"/>
+      <c r="J10" s="156"/>
+      <c r="K10" s="156"/>
+      <c r="L10" s="156"/>
+      <c r="M10" s="156"/>
+      <c r="N10" s="156"/>
+      <c r="O10" s="156"/>
+      <c r="P10" s="156"/>
+      <c r="Q10" s="156"/>
+      <c r="R10" s="156"/>
+      <c r="S10" s="156"/>
+      <c r="T10" s="156"/>
+      <c r="U10" s="156"/>
+      <c r="V10" s="156"/>
+      <c r="W10" s="156"/>
+      <c r="X10" s="156"/>
+      <c r="Y10" s="156"/>
+      <c r="Z10" s="156"/>
+      <c r="AA10" s="156"/>
+      <c r="AB10" s="156"/>
+      <c r="AC10" s="156"/>
+      <c r="AD10" s="156"/>
+      <c r="AE10" s="156"/>
+      <c r="AF10" s="157"/>
+      <c r="AG10" s="155"/>
       <c r="AI10" s="19" t="s">
         <v>46</v>
       </c>
@@ -2690,7 +2691,7 @@
       <c r="AD11" s="32"/>
       <c r="AE11" s="32"/>
       <c r="AF11" s="33"/>
-      <c r="AG11" s="181"/>
+      <c r="AG11" s="155"/>
     </row>
     <row r="12" spans="2:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="47" t="s">
@@ -2727,7 +2728,7 @@
       <c r="AD12" s="30"/>
       <c r="AE12" s="30"/>
       <c r="AF12" s="31"/>
-      <c r="AG12" s="181"/>
+      <c r="AG12" s="155"/>
     </row>
     <row r="13" spans="2:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="104" t="s">
@@ -2764,17 +2765,17 @@
       <c r="AD13" s="97"/>
       <c r="AE13" s="97"/>
       <c r="AF13" s="102"/>
-      <c r="AG13" s="181"/>
+      <c r="AG13" s="155"/>
     </row>
     <row r="14" spans="2:36" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="163" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="169"/>
-      <c r="E14" s="167"/>
-      <c r="F14" s="165"/>
-      <c r="H14" s="173" t="s">
+      <c r="C14" s="165"/>
+      <c r="D14" s="171"/>
+      <c r="E14" s="169"/>
+      <c r="F14" s="167"/>
+      <c r="H14" s="164" t="s">
         <v>80</v>
       </c>
       <c r="I14" s="96"/>
@@ -2801,15 +2802,15 @@
       <c r="AD14" s="97"/>
       <c r="AE14" s="97"/>
       <c r="AF14" s="102"/>
-      <c r="AG14" s="181"/>
+      <c r="AG14" s="155"/>
     </row>
     <row r="15" spans="2:36" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="164"/>
-      <c r="C15" s="172"/>
-      <c r="D15" s="170"/>
-      <c r="E15" s="168"/>
-      <c r="F15" s="166"/>
-      <c r="H15" s="173"/>
+      <c r="B15" s="163"/>
+      <c r="C15" s="166"/>
+      <c r="D15" s="172"/>
+      <c r="E15" s="170"/>
+      <c r="F15" s="168"/>
+      <c r="H15" s="164"/>
       <c r="I15" s="42"/>
       <c r="J15" s="43"/>
       <c r="K15" s="43"/>
@@ -2834,7 +2835,7 @@
       <c r="AD15" s="38"/>
       <c r="AE15" s="43"/>
       <c r="AF15" s="44"/>
-      <c r="AG15" s="181"/>
+      <c r="AG15" s="155"/>
     </row>
     <row r="16" spans="2:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="46" t="s">
@@ -2871,7 +2872,7 @@
       <c r="AD16" s="32"/>
       <c r="AE16" s="32"/>
       <c r="AF16" s="33"/>
-      <c r="AG16" s="181"/>
+      <c r="AG16" s="155"/>
     </row>
     <row r="17" spans="2:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="46" t="s">
@@ -2908,7 +2909,7 @@
       <c r="AD17" s="30"/>
       <c r="AE17" s="30"/>
       <c r="AF17" s="31"/>
-      <c r="AG17" s="181"/>
+      <c r="AG17" s="155"/>
     </row>
     <row r="18" spans="2:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="46" t="s">
@@ -2945,7 +2946,7 @@
       <c r="AD18" s="30"/>
       <c r="AE18" s="30"/>
       <c r="AF18" s="31"/>
-      <c r="AG18" s="181"/>
+      <c r="AG18" s="155"/>
     </row>
     <row r="19" spans="2:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="46" t="s">
@@ -2982,17 +2983,17 @@
       <c r="AD19" s="30"/>
       <c r="AE19" s="30"/>
       <c r="AF19" s="31"/>
-      <c r="AG19" s="181"/>
+      <c r="AG19" s="155"/>
     </row>
     <row r="20" spans="2:33" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="164" t="s">
+      <c r="B20" s="163" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="171"/>
-      <c r="D20" s="169"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="165"/>
-      <c r="H20" s="164" t="s">
+      <c r="C20" s="165"/>
+      <c r="D20" s="171"/>
+      <c r="E20" s="169"/>
+      <c r="F20" s="167"/>
+      <c r="H20" s="163" t="s">
         <v>66</v>
       </c>
       <c r="I20" s="35"/>
@@ -3019,15 +3020,15 @@
       <c r="AD20" s="32"/>
       <c r="AE20" s="32"/>
       <c r="AF20" s="33"/>
-      <c r="AG20" s="181"/>
+      <c r="AG20" s="155"/>
     </row>
     <row r="21" spans="2:33" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="164"/>
-      <c r="C21" s="172"/>
-      <c r="D21" s="170"/>
-      <c r="E21" s="168"/>
-      <c r="F21" s="166"/>
-      <c r="H21" s="164"/>
+      <c r="B21" s="163"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="172"/>
+      <c r="E21" s="170"/>
+      <c r="F21" s="168"/>
+      <c r="H21" s="163"/>
       <c r="I21" s="35"/>
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
@@ -3052,7 +3053,7 @@
       <c r="AD21" s="32"/>
       <c r="AE21" s="32"/>
       <c r="AF21" s="33"/>
-      <c r="AG21" s="181"/>
+      <c r="AG21" s="155"/>
     </row>
     <row r="22" spans="2:33" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="46" t="s">
@@ -3089,44 +3090,44 @@
       <c r="AD22" s="106"/>
       <c r="AE22" s="106"/>
       <c r="AF22" s="112"/>
-      <c r="AG22" s="181"/>
+      <c r="AG22" s="155"/>
     </row>
     <row r="23" spans="2:33" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="155" t="s">
+      <c r="B23" s="175" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="156"/>
-      <c r="D23" s="156"/>
-      <c r="E23" s="156"/>
-      <c r="F23" s="157"/>
+      <c r="C23" s="176"/>
+      <c r="D23" s="176"/>
+      <c r="E23" s="176"/>
+      <c r="F23" s="177"/>
       <c r="H23" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="151"/>
-      <c r="J23" s="151"/>
-      <c r="K23" s="151"/>
-      <c r="L23" s="151"/>
-      <c r="M23" s="151"/>
-      <c r="N23" s="151"/>
-      <c r="O23" s="151"/>
-      <c r="P23" s="151"/>
-      <c r="Q23" s="151"/>
-      <c r="R23" s="151"/>
-      <c r="S23" s="151"/>
-      <c r="T23" s="151"/>
-      <c r="U23" s="151"/>
-      <c r="V23" s="151"/>
-      <c r="W23" s="151"/>
-      <c r="X23" s="151"/>
-      <c r="Y23" s="151"/>
-      <c r="Z23" s="151"/>
-      <c r="AA23" s="151"/>
-      <c r="AB23" s="151"/>
-      <c r="AC23" s="151"/>
-      <c r="AD23" s="151"/>
-      <c r="AE23" s="151"/>
-      <c r="AF23" s="152"/>
-      <c r="AG23" s="181"/>
+      <c r="I23" s="156"/>
+      <c r="J23" s="156"/>
+      <c r="K23" s="156"/>
+      <c r="L23" s="156"/>
+      <c r="M23" s="156"/>
+      <c r="N23" s="156"/>
+      <c r="O23" s="156"/>
+      <c r="P23" s="156"/>
+      <c r="Q23" s="156"/>
+      <c r="R23" s="156"/>
+      <c r="S23" s="156"/>
+      <c r="T23" s="156"/>
+      <c r="U23" s="156"/>
+      <c r="V23" s="156"/>
+      <c r="W23" s="156"/>
+      <c r="X23" s="156"/>
+      <c r="Y23" s="156"/>
+      <c r="Z23" s="156"/>
+      <c r="AA23" s="156"/>
+      <c r="AB23" s="156"/>
+      <c r="AC23" s="156"/>
+      <c r="AD23" s="156"/>
+      <c r="AE23" s="156"/>
+      <c r="AF23" s="157"/>
+      <c r="AG23" s="155"/>
     </row>
     <row r="24" spans="2:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="45" t="s">
@@ -3163,7 +3164,7 @@
       <c r="AD24" s="43"/>
       <c r="AE24" s="43"/>
       <c r="AF24" s="44"/>
-      <c r="AG24" s="181"/>
+      <c r="AG24" s="155"/>
     </row>
     <row r="25" spans="2:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="45" t="s">
@@ -3200,7 +3201,7 @@
       <c r="AD25" s="32"/>
       <c r="AE25" s="32"/>
       <c r="AF25" s="33"/>
-      <c r="AG25" s="181"/>
+      <c r="AG25" s="155"/>
     </row>
     <row r="26" spans="2:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="45" t="s">
@@ -3237,7 +3238,7 @@
       <c r="AD26" s="30"/>
       <c r="AE26" s="30"/>
       <c r="AF26" s="31"/>
-      <c r="AG26" s="181"/>
+      <c r="AG26" s="155"/>
     </row>
     <row r="27" spans="2:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="45" t="s">
@@ -3274,7 +3275,7 @@
       <c r="AD27" s="32"/>
       <c r="AE27" s="32"/>
       <c r="AF27" s="33"/>
-      <c r="AG27" s="181"/>
+      <c r="AG27" s="155"/>
     </row>
     <row r="28" spans="2:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="45" t="s">
@@ -3311,7 +3312,7 @@
       <c r="AD28" s="30"/>
       <c r="AE28" s="30"/>
       <c r="AF28" s="31"/>
-      <c r="AG28" s="181"/>
+      <c r="AG28" s="155"/>
     </row>
     <row r="29" spans="2:33" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="49" t="s">
@@ -3348,7 +3349,7 @@
       <c r="AD29" s="40"/>
       <c r="AE29" s="40"/>
       <c r="AF29" s="41"/>
-      <c r="AG29" s="181"/>
+      <c r="AG29" s="155"/>
     </row>
     <row r="30" spans="2:33" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="29" t="s">
@@ -3361,33 +3362,33 @@
       <c r="H30" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I30" s="178" t="s">
+      <c r="I30" s="152" t="s">
         <v>79</v>
       </c>
-      <c r="J30" s="179"/>
-      <c r="K30" s="179"/>
-      <c r="L30" s="179"/>
-      <c r="M30" s="179"/>
-      <c r="N30" s="179"/>
-      <c r="O30" s="179"/>
-      <c r="P30" s="179"/>
-      <c r="Q30" s="179"/>
-      <c r="R30" s="179"/>
-      <c r="S30" s="179"/>
-      <c r="T30" s="179"/>
-      <c r="U30" s="179"/>
-      <c r="V30" s="179"/>
-      <c r="W30" s="179"/>
-      <c r="X30" s="179"/>
-      <c r="Y30" s="179"/>
-      <c r="Z30" s="179"/>
-      <c r="AA30" s="179"/>
-      <c r="AB30" s="179"/>
-      <c r="AC30" s="179"/>
-      <c r="AD30" s="179"/>
-      <c r="AE30" s="179"/>
-      <c r="AF30" s="180"/>
-      <c r="AG30" s="181"/>
+      <c r="J30" s="153"/>
+      <c r="K30" s="153"/>
+      <c r="L30" s="153"/>
+      <c r="M30" s="153"/>
+      <c r="N30" s="153"/>
+      <c r="O30" s="153"/>
+      <c r="P30" s="153"/>
+      <c r="Q30" s="153"/>
+      <c r="R30" s="153"/>
+      <c r="S30" s="153"/>
+      <c r="T30" s="153"/>
+      <c r="U30" s="153"/>
+      <c r="V30" s="153"/>
+      <c r="W30" s="153"/>
+      <c r="X30" s="153"/>
+      <c r="Y30" s="153"/>
+      <c r="Z30" s="153"/>
+      <c r="AA30" s="153"/>
+      <c r="AB30" s="153"/>
+      <c r="AC30" s="153"/>
+      <c r="AD30" s="153"/>
+      <c r="AE30" s="153"/>
+      <c r="AF30" s="154"/>
+      <c r="AG30" s="155"/>
     </row>
     <row r="31" spans="2:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3469,75 +3470,75 @@
       <c r="H34" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="I34" s="177">
+      <c r="I34" s="162">
         <v>43049</v>
       </c>
-      <c r="J34" s="175"/>
-      <c r="K34" s="176"/>
-      <c r="L34" s="174">
+      <c r="J34" s="159"/>
+      <c r="K34" s="160"/>
+      <c r="L34" s="158">
         <v>43056</v>
       </c>
-      <c r="M34" s="175"/>
-      <c r="N34" s="176"/>
-      <c r="O34" s="174">
+      <c r="M34" s="159"/>
+      <c r="N34" s="160"/>
+      <c r="O34" s="158">
         <v>43063</v>
       </c>
-      <c r="P34" s="175"/>
-      <c r="Q34" s="176"/>
-      <c r="R34" s="174">
+      <c r="P34" s="159"/>
+      <c r="Q34" s="160"/>
+      <c r="R34" s="158">
         <v>43070</v>
       </c>
-      <c r="S34" s="175"/>
-      <c r="T34" s="176"/>
-      <c r="U34" s="174">
+      <c r="S34" s="159"/>
+      <c r="T34" s="160"/>
+      <c r="U34" s="158">
         <v>43084</v>
       </c>
-      <c r="V34" s="175"/>
-      <c r="W34" s="176"/>
-      <c r="X34" s="174">
+      <c r="V34" s="159"/>
+      <c r="W34" s="160"/>
+      <c r="X34" s="158">
         <v>43091</v>
       </c>
-      <c r="Y34" s="175"/>
-      <c r="Z34" s="176"/>
-      <c r="AA34" s="174">
+      <c r="Y34" s="159"/>
+      <c r="Z34" s="160"/>
+      <c r="AA34" s="158">
         <v>43112</v>
       </c>
-      <c r="AB34" s="175"/>
-      <c r="AC34" s="176"/>
-      <c r="AD34" s="175">
+      <c r="AB34" s="159"/>
+      <c r="AC34" s="160"/>
+      <c r="AD34" s="159">
         <v>43119</v>
       </c>
-      <c r="AE34" s="175"/>
-      <c r="AF34" s="182"/>
+      <c r="AE34" s="159"/>
+      <c r="AF34" s="161"/>
     </row>
     <row r="35" spans="8:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H35" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="I35" s="151"/>
-      <c r="J35" s="151"/>
-      <c r="K35" s="151"/>
-      <c r="L35" s="151"/>
-      <c r="M35" s="151"/>
-      <c r="N35" s="151"/>
-      <c r="O35" s="151"/>
-      <c r="P35" s="151"/>
-      <c r="Q35" s="151"/>
-      <c r="R35" s="151"/>
-      <c r="S35" s="151"/>
-      <c r="T35" s="151"/>
-      <c r="U35" s="151"/>
-      <c r="V35" s="151"/>
-      <c r="W35" s="151"/>
-      <c r="X35" s="151"/>
-      <c r="Y35" s="151"/>
-      <c r="Z35" s="151"/>
-      <c r="AA35" s="151"/>
-      <c r="AB35" s="151"/>
-      <c r="AC35" s="151"/>
-      <c r="AD35" s="151"/>
-      <c r="AE35" s="151"/>
-      <c r="AF35" s="152"/>
+      <c r="I35" s="156"/>
+      <c r="J35" s="156"/>
+      <c r="K35" s="156"/>
+      <c r="L35" s="156"/>
+      <c r="M35" s="156"/>
+      <c r="N35" s="156"/>
+      <c r="O35" s="156"/>
+      <c r="P35" s="156"/>
+      <c r="Q35" s="156"/>
+      <c r="R35" s="156"/>
+      <c r="S35" s="156"/>
+      <c r="T35" s="156"/>
+      <c r="U35" s="156"/>
+      <c r="V35" s="156"/>
+      <c r="W35" s="156"/>
+      <c r="X35" s="156"/>
+      <c r="Y35" s="156"/>
+      <c r="Z35" s="156"/>
+      <c r="AA35" s="156"/>
+      <c r="AB35" s="156"/>
+      <c r="AC35" s="156"/>
+      <c r="AD35" s="156"/>
+      <c r="AE35" s="156"/>
+      <c r="AF35" s="157"/>
     </row>
     <row r="36" spans="8:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H36" s="26" t="s">
@@ -3630,30 +3631,30 @@
       <c r="H39" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="I39" s="151"/>
-      <c r="J39" s="151"/>
-      <c r="K39" s="151"/>
-      <c r="L39" s="151"/>
-      <c r="M39" s="151"/>
-      <c r="N39" s="151"/>
-      <c r="O39" s="151"/>
-      <c r="P39" s="151"/>
-      <c r="Q39" s="151"/>
-      <c r="R39" s="151"/>
-      <c r="S39" s="151"/>
-      <c r="T39" s="151"/>
-      <c r="U39" s="151"/>
-      <c r="V39" s="151"/>
-      <c r="W39" s="151"/>
-      <c r="X39" s="151"/>
-      <c r="Y39" s="151"/>
-      <c r="Z39" s="151"/>
-      <c r="AA39" s="151"/>
-      <c r="AB39" s="151"/>
-      <c r="AC39" s="151"/>
-      <c r="AD39" s="151"/>
-      <c r="AE39" s="151"/>
-      <c r="AF39" s="152"/>
+      <c r="I39" s="156"/>
+      <c r="J39" s="156"/>
+      <c r="K39" s="156"/>
+      <c r="L39" s="156"/>
+      <c r="M39" s="156"/>
+      <c r="N39" s="156"/>
+      <c r="O39" s="156"/>
+      <c r="P39" s="156"/>
+      <c r="Q39" s="156"/>
+      <c r="R39" s="156"/>
+      <c r="S39" s="156"/>
+      <c r="T39" s="156"/>
+      <c r="U39" s="156"/>
+      <c r="V39" s="156"/>
+      <c r="W39" s="156"/>
+      <c r="X39" s="156"/>
+      <c r="Y39" s="156"/>
+      <c r="Z39" s="156"/>
+      <c r="AA39" s="156"/>
+      <c r="AB39" s="156"/>
+      <c r="AC39" s="156"/>
+      <c r="AD39" s="156"/>
+      <c r="AE39" s="156"/>
+      <c r="AF39" s="157"/>
     </row>
     <row r="40" spans="8:32" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H40" s="26" t="s">
@@ -3688,30 +3689,30 @@
       <c r="H41" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="I41" s="151"/>
-      <c r="J41" s="151"/>
-      <c r="K41" s="151"/>
-      <c r="L41" s="151"/>
-      <c r="M41" s="151"/>
-      <c r="N41" s="151"/>
-      <c r="O41" s="151"/>
-      <c r="P41" s="151"/>
-      <c r="Q41" s="151"/>
-      <c r="R41" s="151"/>
-      <c r="S41" s="151"/>
-      <c r="T41" s="151"/>
-      <c r="U41" s="151"/>
-      <c r="V41" s="151"/>
-      <c r="W41" s="151"/>
-      <c r="X41" s="151"/>
-      <c r="Y41" s="151"/>
-      <c r="Z41" s="151"/>
-      <c r="AA41" s="151"/>
-      <c r="AB41" s="151"/>
-      <c r="AC41" s="151"/>
-      <c r="AD41" s="151"/>
-      <c r="AE41" s="151"/>
-      <c r="AF41" s="152"/>
+      <c r="I41" s="156"/>
+      <c r="J41" s="156"/>
+      <c r="K41" s="156"/>
+      <c r="L41" s="156"/>
+      <c r="M41" s="156"/>
+      <c r="N41" s="156"/>
+      <c r="O41" s="156"/>
+      <c r="P41" s="156"/>
+      <c r="Q41" s="156"/>
+      <c r="R41" s="156"/>
+      <c r="S41" s="156"/>
+      <c r="T41" s="156"/>
+      <c r="U41" s="156"/>
+      <c r="V41" s="156"/>
+      <c r="W41" s="156"/>
+      <c r="X41" s="156"/>
+      <c r="Y41" s="156"/>
+      <c r="Z41" s="156"/>
+      <c r="AA41" s="156"/>
+      <c r="AB41" s="156"/>
+      <c r="AC41" s="156"/>
+      <c r="AD41" s="156"/>
+      <c r="AE41" s="156"/>
+      <c r="AF41" s="157"/>
     </row>
     <row r="42" spans="8:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H42" s="16" t="s">
@@ -3801,7 +3802,7 @@
       <c r="AF44" s="102"/>
     </row>
     <row r="45" spans="8:32" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H45" s="173" t="s">
+      <c r="H45" s="164" t="s">
         <v>80</v>
       </c>
       <c r="I45" s="96"/>
@@ -3819,9 +3820,9 @@
       <c r="U45" s="126"/>
       <c r="V45" s="99"/>
       <c r="W45" s="100"/>
-      <c r="X45" s="98"/>
-      <c r="Y45" s="97"/>
-      <c r="Z45" s="101"/>
+      <c r="X45" s="126"/>
+      <c r="Y45" s="99"/>
+      <c r="Z45" s="100"/>
       <c r="AA45" s="98"/>
       <c r="AB45" s="97"/>
       <c r="AC45" s="101"/>
@@ -3830,7 +3831,7 @@
       <c r="AF45" s="102"/>
     </row>
     <row r="46" spans="8:32" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H46" s="173"/>
+      <c r="H46" s="164"/>
       <c r="I46" s="42"/>
       <c r="J46" s="43"/>
       <c r="K46" s="43"/>
@@ -3844,11 +3845,11 @@
       <c r="S46" s="113"/>
       <c r="T46" s="113"/>
       <c r="U46" s="114"/>
-      <c r="V46" s="43"/>
-      <c r="W46" s="43"/>
-      <c r="X46" s="38"/>
-      <c r="Y46" s="43"/>
-      <c r="Z46" s="43"/>
+      <c r="V46" s="113"/>
+      <c r="W46" s="184"/>
+      <c r="X46" s="114"/>
+      <c r="Y46" s="113"/>
+      <c r="Z46" s="184"/>
       <c r="AA46" s="38"/>
       <c r="AB46" s="43"/>
       <c r="AC46" s="43"/>
@@ -3875,9 +3876,9 @@
       <c r="U47" s="80"/>
       <c r="V47" s="80"/>
       <c r="W47" s="32"/>
-      <c r="X47" s="53"/>
-      <c r="Y47" s="32"/>
-      <c r="Z47" s="50"/>
+      <c r="X47" s="87"/>
+      <c r="Y47" s="87"/>
+      <c r="Z47" s="87"/>
       <c r="AA47" s="53"/>
       <c r="AB47" s="32"/>
       <c r="AC47" s="50"/>
@@ -3903,7 +3904,7 @@
       <c r="T48" s="37"/>
       <c r="U48" s="30"/>
       <c r="V48" s="30"/>
-      <c r="W48" s="183"/>
+      <c r="W48" s="127"/>
       <c r="X48" s="36"/>
       <c r="Y48" s="30"/>
       <c r="Z48" s="37"/>
@@ -3973,7 +3974,7 @@
       <c r="AF50" s="31"/>
     </row>
     <row r="51" spans="8:32" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H51" s="164" t="s">
+      <c r="H51" s="163" t="s">
         <v>66</v>
       </c>
       <c r="I51" s="35"/>
@@ -4002,7 +4003,7 @@
       <c r="AF51" s="33"/>
     </row>
     <row r="52" spans="8:32" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H52" s="164"/>
+      <c r="H52" s="163"/>
       <c r="I52" s="35"/>
       <c r="J52" s="32"/>
       <c r="K52" s="32"/>
@@ -4061,30 +4062,30 @@
       <c r="H54" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="I54" s="151"/>
-      <c r="J54" s="151"/>
-      <c r="K54" s="151"/>
-      <c r="L54" s="151"/>
-      <c r="M54" s="151"/>
-      <c r="N54" s="151"/>
-      <c r="O54" s="151"/>
-      <c r="P54" s="151"/>
-      <c r="Q54" s="151"/>
-      <c r="R54" s="151"/>
-      <c r="S54" s="151"/>
-      <c r="T54" s="151"/>
-      <c r="U54" s="151"/>
-      <c r="V54" s="151"/>
-      <c r="W54" s="151"/>
-      <c r="X54" s="151"/>
-      <c r="Y54" s="151"/>
-      <c r="Z54" s="151"/>
-      <c r="AA54" s="151"/>
-      <c r="AB54" s="151"/>
-      <c r="AC54" s="151"/>
-      <c r="AD54" s="151"/>
-      <c r="AE54" s="151"/>
-      <c r="AF54" s="152"/>
+      <c r="I54" s="156"/>
+      <c r="J54" s="156"/>
+      <c r="K54" s="156"/>
+      <c r="L54" s="156"/>
+      <c r="M54" s="156"/>
+      <c r="N54" s="156"/>
+      <c r="O54" s="156"/>
+      <c r="P54" s="156"/>
+      <c r="Q54" s="156"/>
+      <c r="R54" s="156"/>
+      <c r="S54" s="156"/>
+      <c r="T54" s="156"/>
+      <c r="U54" s="156"/>
+      <c r="V54" s="156"/>
+      <c r="W54" s="156"/>
+      <c r="X54" s="156"/>
+      <c r="Y54" s="156"/>
+      <c r="Z54" s="156"/>
+      <c r="AA54" s="156"/>
+      <c r="AB54" s="156"/>
+      <c r="AC54" s="156"/>
+      <c r="AD54" s="156"/>
+      <c r="AE54" s="156"/>
+      <c r="AF54" s="157"/>
     </row>
     <row r="55" spans="8:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H55" s="45" t="s">
@@ -4264,32 +4265,32 @@
       <c r="H61" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I61" s="178" t="s">
+      <c r="I61" s="152" t="s">
         <v>79</v>
       </c>
-      <c r="J61" s="179"/>
-      <c r="K61" s="179"/>
-      <c r="L61" s="179"/>
-      <c r="M61" s="179"/>
-      <c r="N61" s="179"/>
-      <c r="O61" s="179"/>
-      <c r="P61" s="179"/>
-      <c r="Q61" s="179"/>
-      <c r="R61" s="179"/>
-      <c r="S61" s="179"/>
-      <c r="T61" s="179"/>
-      <c r="U61" s="179"/>
-      <c r="V61" s="179"/>
-      <c r="W61" s="179"/>
-      <c r="X61" s="179"/>
-      <c r="Y61" s="179"/>
-      <c r="Z61" s="179"/>
-      <c r="AA61" s="179"/>
-      <c r="AB61" s="179"/>
-      <c r="AC61" s="179"/>
-      <c r="AD61" s="179"/>
-      <c r="AE61" s="179"/>
-      <c r="AF61" s="180"/>
+      <c r="J61" s="153"/>
+      <c r="K61" s="153"/>
+      <c r="L61" s="153"/>
+      <c r="M61" s="153"/>
+      <c r="N61" s="153"/>
+      <c r="O61" s="153"/>
+      <c r="P61" s="153"/>
+      <c r="Q61" s="153"/>
+      <c r="R61" s="153"/>
+      <c r="S61" s="153"/>
+      <c r="T61" s="153"/>
+      <c r="U61" s="153"/>
+      <c r="V61" s="153"/>
+      <c r="W61" s="153"/>
+      <c r="X61" s="153"/>
+      <c r="Y61" s="153"/>
+      <c r="Z61" s="153"/>
+      <c r="AA61" s="153"/>
+      <c r="AB61" s="153"/>
+      <c r="AC61" s="153"/>
+      <c r="AD61" s="153"/>
+      <c r="AE61" s="153"/>
+      <c r="AF61" s="154"/>
     </row>
     <row r="62" spans="8:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="8:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4312,6 +4313,36 @@
     <row r="78" spans="30:30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="I4:AF4"/>
+    <mergeCell ref="I8:AF8"/>
+    <mergeCell ref="I23:AF23"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="I10:AF10"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="U34:W34"/>
+    <mergeCell ref="X34:Z34"/>
+    <mergeCell ref="I54:AF54"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="H45:H46"/>
     <mergeCell ref="I61:AF61"/>
     <mergeCell ref="AG2:AG30"/>
     <mergeCell ref="I35:AF35"/>
@@ -4328,36 +4359,6 @@
     <mergeCell ref="AD3:AF3"/>
     <mergeCell ref="AA3:AC3"/>
     <mergeCell ref="I30:AF30"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="U34:W34"/>
-    <mergeCell ref="X34:Z34"/>
-    <mergeCell ref="I54:AF54"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="I4:AF4"/>
-    <mergeCell ref="I8:AF8"/>
-    <mergeCell ref="I23:AF23"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="I10:AF10"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>